<commit_message>
created main.py, unlimited playlist length now
</commit_message>
<xml_diff>
--- a/duplicates_mask.xlsx
+++ b/duplicates_mask.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B895"/>
+  <dimension ref="A1:B726"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -2091,7 +2091,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -2131,7 +2131,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214">
@@ -2139,7 +2139,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -2171,7 +2171,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -2179,7 +2179,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -2187,7 +2187,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -2195,7 +2195,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
@@ -2203,7 +2203,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -2243,7 +2243,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228">
@@ -2251,7 +2251,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -2259,7 +2259,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -2291,7 +2291,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -2363,7 +2363,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243">
@@ -2379,7 +2379,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -2475,7 +2475,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -2531,7 +2531,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264">
@@ -2539,7 +2539,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265">
@@ -2555,7 +2555,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -2571,7 +2571,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -2587,7 +2587,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
@@ -2603,7 +2603,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
@@ -2611,7 +2611,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274">
@@ -2619,7 +2619,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275">
@@ -2635,7 +2635,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277">
@@ -2643,7 +2643,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278">
@@ -2651,7 +2651,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -2747,7 +2747,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291">
@@ -2859,7 +2859,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305">
@@ -2867,7 +2867,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306">
@@ -2875,7 +2875,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307">
@@ -2883,7 +2883,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="308">
@@ -2899,7 +2899,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310">
@@ -2907,7 +2907,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311">
@@ -2915,7 +2915,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="312">
@@ -2931,7 +2931,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="314">
@@ -2947,7 +2947,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="316">
@@ -2955,7 +2955,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317">
@@ -2963,7 +2963,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318">
@@ -3027,7 +3027,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -3035,7 +3035,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327">
@@ -3043,7 +3043,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328">
@@ -3051,7 +3051,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329">
@@ -3059,7 +3059,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330">
@@ -3067,7 +3067,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331">
@@ -3075,7 +3075,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332">
@@ -3091,7 +3091,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334">
@@ -3099,7 +3099,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335">
@@ -3107,7 +3107,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336">
@@ -3115,7 +3115,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="337">
@@ -3155,7 +3155,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342">
@@ -3163,7 +3163,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343">
@@ -3171,7 +3171,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344">
@@ -3179,7 +3179,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345">
@@ -3235,7 +3235,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352">
@@ -3243,7 +3243,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="353">
@@ -3259,7 +3259,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355">
@@ -3291,7 +3291,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359">
@@ -3299,7 +3299,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="360">
@@ -3323,7 +3323,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363">
@@ -3339,7 +3339,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365">
@@ -3355,7 +3355,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367">
@@ -3363,7 +3363,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368">
@@ -3379,7 +3379,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370">
@@ -3387,7 +3387,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371">
@@ -3403,7 +3403,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373">
@@ -3427,7 +3427,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376">
@@ -3435,7 +3435,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377">
@@ -3443,7 +3443,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378">
@@ -3451,7 +3451,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="379">
@@ -3459,7 +3459,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="380">
@@ -3467,7 +3467,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381">
@@ -3475,7 +3475,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
@@ -3483,7 +3483,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="383">
@@ -3491,7 +3491,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384">
@@ -3499,7 +3499,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385">
@@ -3507,7 +3507,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="386">
@@ -3515,7 +3515,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="387">
@@ -3523,7 +3523,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388">
@@ -3531,7 +3531,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389">
@@ -3539,7 +3539,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="390">
@@ -3547,7 +3547,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391">
@@ -3555,7 +3555,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392">
@@ -3563,7 +3563,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="393">
@@ -3571,7 +3571,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
@@ -3579,7 +3579,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395">
@@ -3587,7 +3587,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396">
@@ -3595,7 +3595,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397">
@@ -3603,7 +3603,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="398">
@@ -3611,7 +3611,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="399">
@@ -3619,7 +3619,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400">
@@ -3627,7 +3627,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="401">
@@ -3635,7 +3635,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="402">
@@ -3643,7 +3643,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="403">
@@ -3651,7 +3651,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="404">
@@ -3803,7 +3803,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423">
@@ -3819,7 +3819,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="425">
@@ -3843,7 +3843,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="428">
@@ -3883,7 +3883,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433">
@@ -3899,7 +3899,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="435">
@@ -3907,7 +3907,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="436">
@@ -3923,7 +3923,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="438">
@@ -3931,7 +3931,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439">
@@ -3939,7 +3939,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440">
@@ -3947,7 +3947,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441">
@@ -3955,7 +3955,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442">
@@ -3963,7 +3963,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443">
@@ -3971,7 +3971,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="444">
@@ -4011,7 +4011,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449">
@@ -4019,7 +4019,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450">
@@ -4067,7 +4067,7 @@
         <v>453</v>
       </c>
       <c r="B455" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="456">
@@ -4083,7 +4083,7 @@
         <v>455</v>
       </c>
       <c r="B457" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="458">
@@ -4091,7 +4091,7 @@
         <v>456</v>
       </c>
       <c r="B458" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459">
@@ -4099,7 +4099,7 @@
         <v>457</v>
       </c>
       <c r="B459" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="460">
@@ -4107,7 +4107,7 @@
         <v>458</v>
       </c>
       <c r="B460" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="461">
@@ -4115,7 +4115,7 @@
         <v>459</v>
       </c>
       <c r="B461" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="462">
@@ -4131,7 +4131,7 @@
         <v>461</v>
       </c>
       <c r="B463" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="464">
@@ -4139,7 +4139,7 @@
         <v>462</v>
       </c>
       <c r="B464" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="465">
@@ -4147,7 +4147,7 @@
         <v>463</v>
       </c>
       <c r="B465" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="466">
@@ -4171,7 +4171,7 @@
         <v>466</v>
       </c>
       <c r="B468" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="469">
@@ -4187,7 +4187,7 @@
         <v>468</v>
       </c>
       <c r="B470" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471">
@@ -4211,7 +4211,7 @@
         <v>471</v>
       </c>
       <c r="B473" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="474">
@@ -4219,7 +4219,7 @@
         <v>472</v>
       </c>
       <c r="B474" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="475">
@@ -4323,7 +4323,7 @@
         <v>485</v>
       </c>
       <c r="B487" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="488">
@@ -4331,7 +4331,7 @@
         <v>486</v>
       </c>
       <c r="B488" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="489">
@@ -4355,7 +4355,7 @@
         <v>489</v>
       </c>
       <c r="B491" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="492">
@@ -4363,7 +4363,7 @@
         <v>490</v>
       </c>
       <c r="B492" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="493">
@@ -4371,7 +4371,7 @@
         <v>491</v>
       </c>
       <c r="B493" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="494">
@@ -4379,7 +4379,7 @@
         <v>492</v>
       </c>
       <c r="B494" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="495">
@@ -4443,7 +4443,7 @@
         <v>500</v>
       </c>
       <c r="B502" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="503">
@@ -4539,7 +4539,7 @@
         <v>512</v>
       </c>
       <c r="B514" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="515">
@@ -4547,7 +4547,7 @@
         <v>513</v>
       </c>
       <c r="B515" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="516">
@@ -4595,7 +4595,7 @@
         <v>519</v>
       </c>
       <c r="B521" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="522">
@@ -4619,7 +4619,7 @@
         <v>522</v>
       </c>
       <c r="B524" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="525">
@@ -4627,7 +4627,7 @@
         <v>523</v>
       </c>
       <c r="B525" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="526">
@@ -4643,7 +4643,7 @@
         <v>525</v>
       </c>
       <c r="B527" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="528">
@@ -4699,7 +4699,7 @@
         <v>532</v>
       </c>
       <c r="B534" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="535">
@@ -4707,7 +4707,7 @@
         <v>533</v>
       </c>
       <c r="B535" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="536">
@@ -4731,7 +4731,7 @@
         <v>536</v>
       </c>
       <c r="B538" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="539">
@@ -4739,7 +4739,7 @@
         <v>537</v>
       </c>
       <c r="B539" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="540">
@@ -4755,7 +4755,7 @@
         <v>539</v>
       </c>
       <c r="B541" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="542">
@@ -4779,7 +4779,7 @@
         <v>542</v>
       </c>
       <c r="B544" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="545">
@@ -4787,7 +4787,7 @@
         <v>543</v>
       </c>
       <c r="B545" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="546">
@@ -4811,7 +4811,7 @@
         <v>546</v>
       </c>
       <c r="B548" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="549">
@@ -4891,7 +4891,7 @@
         <v>556</v>
       </c>
       <c r="B558" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="559">
@@ -4899,7 +4899,7 @@
         <v>557</v>
       </c>
       <c r="B559" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="560">
@@ -4915,7 +4915,7 @@
         <v>559</v>
       </c>
       <c r="B561" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="562">
@@ -4963,7 +4963,7 @@
         <v>565</v>
       </c>
       <c r="B567" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="568">
@@ -5003,7 +5003,7 @@
         <v>570</v>
       </c>
       <c r="B572" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="573">
@@ -5011,7 +5011,7 @@
         <v>571</v>
       </c>
       <c r="B573" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="574">
@@ -5019,7 +5019,7 @@
         <v>572</v>
       </c>
       <c r="B574" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="575">
@@ -5035,7 +5035,7 @@
         <v>574</v>
       </c>
       <c r="B576" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="577">
@@ -5083,7 +5083,7 @@
         <v>580</v>
       </c>
       <c r="B582" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="583">
@@ -5091,7 +5091,7 @@
         <v>581</v>
       </c>
       <c r="B583" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="584">
@@ -5107,7 +5107,7 @@
         <v>583</v>
       </c>
       <c r="B585" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="586">
@@ -5123,7 +5123,7 @@
         <v>585</v>
       </c>
       <c r="B587" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="588">
@@ -5147,7 +5147,7 @@
         <v>588</v>
       </c>
       <c r="B590" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="591">
@@ -5195,7 +5195,7 @@
         <v>594</v>
       </c>
       <c r="B596" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="597">
@@ -5219,7 +5219,7 @@
         <v>597</v>
       </c>
       <c r="B599" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="600">
@@ -5267,7 +5267,7 @@
         <v>603</v>
       </c>
       <c r="B605" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="606">
@@ -5283,7 +5283,7 @@
         <v>605</v>
       </c>
       <c r="B607" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="608">
@@ -5299,7 +5299,7 @@
         <v>607</v>
       </c>
       <c r="B609" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="610">
@@ -5307,7 +5307,7 @@
         <v>608</v>
       </c>
       <c r="B610" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="611">
@@ -5315,7 +5315,7 @@
         <v>609</v>
       </c>
       <c r="B611" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="612">
@@ -5363,7 +5363,7 @@
         <v>615</v>
       </c>
       <c r="B617" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="618">
@@ -5371,7 +5371,7 @@
         <v>616</v>
       </c>
       <c r="B618" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="619">
@@ -5379,7 +5379,7 @@
         <v>617</v>
       </c>
       <c r="B619" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="620">
@@ -5395,7 +5395,7 @@
         <v>619</v>
       </c>
       <c r="B621" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="622">
@@ -5403,7 +5403,7 @@
         <v>620</v>
       </c>
       <c r="B622" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="623">
@@ -5411,7 +5411,7 @@
         <v>621</v>
       </c>
       <c r="B623" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="624">
@@ -5419,7 +5419,7 @@
         <v>622</v>
       </c>
       <c r="B624" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="625">
@@ -5435,7 +5435,7 @@
         <v>624</v>
       </c>
       <c r="B626" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="627">
@@ -5451,7 +5451,7 @@
         <v>626</v>
       </c>
       <c r="B628" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="629">
@@ -5459,7 +5459,7 @@
         <v>627</v>
       </c>
       <c r="B629" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="630">
@@ -5475,7 +5475,7 @@
         <v>629</v>
       </c>
       <c r="B631" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="632">
@@ -5483,7 +5483,7 @@
         <v>630</v>
       </c>
       <c r="B632" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="633">
@@ -5499,7 +5499,7 @@
         <v>632</v>
       </c>
       <c r="B634" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="635">
@@ -5507,7 +5507,7 @@
         <v>633</v>
       </c>
       <c r="B635" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="636">
@@ -5523,7 +5523,7 @@
         <v>635</v>
       </c>
       <c r="B637" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="638">
@@ -5531,7 +5531,7 @@
         <v>636</v>
       </c>
       <c r="B638" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="639">
@@ -5539,7 +5539,7 @@
         <v>637</v>
       </c>
       <c r="B639" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="640">
@@ -5547,7 +5547,7 @@
         <v>638</v>
       </c>
       <c r="B640" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="641">
@@ -5587,7 +5587,7 @@
         <v>643</v>
       </c>
       <c r="B645" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="646">
@@ -5659,7 +5659,7 @@
         <v>652</v>
       </c>
       <c r="B654" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="655">
@@ -5667,7 +5667,7 @@
         <v>653</v>
       </c>
       <c r="B655" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="656">
@@ -5715,7 +5715,7 @@
         <v>659</v>
       </c>
       <c r="B661" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="662">
@@ -5723,7 +5723,7 @@
         <v>660</v>
       </c>
       <c r="B662" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="663">
@@ -5739,7 +5739,7 @@
         <v>662</v>
       </c>
       <c r="B664" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="665">
@@ -5755,7 +5755,7 @@
         <v>664</v>
       </c>
       <c r="B666" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="667">
@@ -5779,7 +5779,7 @@
         <v>667</v>
       </c>
       <c r="B669" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="670">
@@ -5787,7 +5787,7 @@
         <v>668</v>
       </c>
       <c r="B670" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="671">
@@ -5803,7 +5803,7 @@
         <v>670</v>
       </c>
       <c r="B672" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="673">
@@ -5819,7 +5819,7 @@
         <v>672</v>
       </c>
       <c r="B674" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="675">
@@ -5827,7 +5827,7 @@
         <v>673</v>
       </c>
       <c r="B675" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="676">
@@ -5835,7 +5835,7 @@
         <v>674</v>
       </c>
       <c r="B676" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="677">
@@ -5843,7 +5843,7 @@
         <v>675</v>
       </c>
       <c r="B677" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="678">
@@ -5851,7 +5851,7 @@
         <v>676</v>
       </c>
       <c r="B678" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="679">
@@ -5859,7 +5859,7 @@
         <v>677</v>
       </c>
       <c r="B679" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="680">
@@ -5867,7 +5867,7 @@
         <v>678</v>
       </c>
       <c r="B680" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="681">
@@ -5875,7 +5875,7 @@
         <v>679</v>
       </c>
       <c r="B681" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="682">
@@ -5883,7 +5883,7 @@
         <v>680</v>
       </c>
       <c r="B682" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="683">
@@ -5899,7 +5899,7 @@
         <v>682</v>
       </c>
       <c r="B684" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="685">
@@ -5915,7 +5915,7 @@
         <v>684</v>
       </c>
       <c r="B686" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="687">
@@ -5939,7 +5939,7 @@
         <v>687</v>
       </c>
       <c r="B689" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="690">
@@ -5947,7 +5947,7 @@
         <v>688</v>
       </c>
       <c r="B690" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="691">
@@ -5955,7 +5955,7 @@
         <v>689</v>
       </c>
       <c r="B691" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="692">
@@ -5963,7 +5963,7 @@
         <v>690</v>
       </c>
       <c r="B692" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="693">
@@ -5987,7 +5987,7 @@
         <v>693</v>
       </c>
       <c r="B695" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="696">
@@ -5995,7 +5995,7 @@
         <v>694</v>
       </c>
       <c r="B696" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="697">
@@ -6003,7 +6003,7 @@
         <v>695</v>
       </c>
       <c r="B697" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="698">
@@ -6019,7 +6019,7 @@
         <v>697</v>
       </c>
       <c r="B699" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="700">
@@ -6035,7 +6035,7 @@
         <v>699</v>
       </c>
       <c r="B701" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="702">
@@ -6051,7 +6051,7 @@
         <v>701</v>
       </c>
       <c r="B703" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="704">
@@ -6059,7 +6059,7 @@
         <v>702</v>
       </c>
       <c r="B704" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="705">
@@ -6075,7 +6075,7 @@
         <v>704</v>
       </c>
       <c r="B706" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="707">
@@ -6083,7 +6083,7 @@
         <v>705</v>
       </c>
       <c r="B707" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="708">
@@ -6091,7 +6091,7 @@
         <v>706</v>
       </c>
       <c r="B708" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="709">
@@ -6099,7 +6099,7 @@
         <v>707</v>
       </c>
       <c r="B709" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="710">
@@ -6107,7 +6107,7 @@
         <v>708</v>
       </c>
       <c r="B710" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="711">
@@ -6115,7 +6115,7 @@
         <v>709</v>
       </c>
       <c r="B711" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="712">
@@ -6123,7 +6123,7 @@
         <v>710</v>
       </c>
       <c r="B712" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="713">
@@ -6131,7 +6131,7 @@
         <v>711</v>
       </c>
       <c r="B713" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="714">
@@ -6139,7 +6139,7 @@
         <v>712</v>
       </c>
       <c r="B714" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="715">
@@ -6147,7 +6147,7 @@
         <v>713</v>
       </c>
       <c r="B715" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="716">
@@ -6155,7 +6155,7 @@
         <v>714</v>
       </c>
       <c r="B716" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="717">
@@ -6163,7 +6163,7 @@
         <v>715</v>
       </c>
       <c r="B717" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="718">
@@ -6171,7 +6171,7 @@
         <v>716</v>
       </c>
       <c r="B718" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="719">
@@ -6211,7 +6211,7 @@
         <v>721</v>
       </c>
       <c r="B723" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="724">
@@ -6219,7 +6219,7 @@
         <v>722</v>
       </c>
       <c r="B724" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="725">
@@ -6235,1359 +6235,7 @@
         <v>724</v>
       </c>
       <c r="B726" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="727">
-      <c r="A727" s="1" t="n">
-        <v>725</v>
-      </c>
-      <c r="B727" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="728">
-      <c r="A728" s="1" t="n">
-        <v>726</v>
-      </c>
-      <c r="B728" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="729">
-      <c r="A729" s="1" t="n">
-        <v>727</v>
-      </c>
-      <c r="B729" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="730">
-      <c r="A730" s="1" t="n">
-        <v>728</v>
-      </c>
-      <c r="B730" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="731">
-      <c r="A731" s="1" t="n">
-        <v>729</v>
-      </c>
-      <c r="B731" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="732">
-      <c r="A732" s="1" t="n">
-        <v>730</v>
-      </c>
-      <c r="B732" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="733">
-      <c r="A733" s="1" t="n">
-        <v>731</v>
-      </c>
-      <c r="B733" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="734">
-      <c r="A734" s="1" t="n">
-        <v>732</v>
-      </c>
-      <c r="B734" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="735">
-      <c r="A735" s="1" t="n">
-        <v>733</v>
-      </c>
-      <c r="B735" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="736">
-      <c r="A736" s="1" t="n">
-        <v>734</v>
-      </c>
-      <c r="B736" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="737">
-      <c r="A737" s="1" t="n">
-        <v>735</v>
-      </c>
-      <c r="B737" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="738">
-      <c r="A738" s="1" t="n">
-        <v>736</v>
-      </c>
-      <c r="B738" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="739">
-      <c r="A739" s="1" t="n">
-        <v>737</v>
-      </c>
-      <c r="B739" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="740">
-      <c r="A740" s="1" t="n">
-        <v>738</v>
-      </c>
-      <c r="B740" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="741">
-      <c r="A741" s="1" t="n">
-        <v>739</v>
-      </c>
-      <c r="B741" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="742">
-      <c r="A742" s="1" t="n">
-        <v>740</v>
-      </c>
-      <c r="B742" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="743">
-      <c r="A743" s="1" t="n">
-        <v>741</v>
-      </c>
-      <c r="B743" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="744">
-      <c r="A744" s="1" t="n">
-        <v>742</v>
-      </c>
-      <c r="B744" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="745">
-      <c r="A745" s="1" t="n">
-        <v>743</v>
-      </c>
-      <c r="B745" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="746">
-      <c r="A746" s="1" t="n">
-        <v>744</v>
-      </c>
-      <c r="B746" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="747">
-      <c r="A747" s="1" t="n">
-        <v>745</v>
-      </c>
-      <c r="B747" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="748">
-      <c r="A748" s="1" t="n">
-        <v>746</v>
-      </c>
-      <c r="B748" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="749">
-      <c r="A749" s="1" t="n">
-        <v>747</v>
-      </c>
-      <c r="B749" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="750">
-      <c r="A750" s="1" t="n">
-        <v>748</v>
-      </c>
-      <c r="B750" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="751">
-      <c r="A751" s="1" t="n">
-        <v>749</v>
-      </c>
-      <c r="B751" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="752">
-      <c r="A752" s="1" t="n">
-        <v>750</v>
-      </c>
-      <c r="B752" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="753">
-      <c r="A753" s="1" t="n">
-        <v>751</v>
-      </c>
-      <c r="B753" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="754">
-      <c r="A754" s="1" t="n">
-        <v>752</v>
-      </c>
-      <c r="B754" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="755">
-      <c r="A755" s="1" t="n">
-        <v>753</v>
-      </c>
-      <c r="B755" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="756">
-      <c r="A756" s="1" t="n">
-        <v>754</v>
-      </c>
-      <c r="B756" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="757">
-      <c r="A757" s="1" t="n">
-        <v>755</v>
-      </c>
-      <c r="B757" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="758">
-      <c r="A758" s="1" t="n">
-        <v>756</v>
-      </c>
-      <c r="B758" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="759">
-      <c r="A759" s="1" t="n">
-        <v>757</v>
-      </c>
-      <c r="B759" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="760">
-      <c r="A760" s="1" t="n">
-        <v>758</v>
-      </c>
-      <c r="B760" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="761">
-      <c r="A761" s="1" t="n">
-        <v>759</v>
-      </c>
-      <c r="B761" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="762">
-      <c r="A762" s="1" t="n">
-        <v>760</v>
-      </c>
-      <c r="B762" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="763">
-      <c r="A763" s="1" t="n">
-        <v>761</v>
-      </c>
-      <c r="B763" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="764">
-      <c r="A764" s="1" t="n">
-        <v>762</v>
-      </c>
-      <c r="B764" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="765">
-      <c r="A765" s="1" t="n">
-        <v>763</v>
-      </c>
-      <c r="B765" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="766">
-      <c r="A766" s="1" t="n">
-        <v>764</v>
-      </c>
-      <c r="B766" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="767">
-      <c r="A767" s="1" t="n">
-        <v>765</v>
-      </c>
-      <c r="B767" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="768">
-      <c r="A768" s="1" t="n">
-        <v>766</v>
-      </c>
-      <c r="B768" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="769">
-      <c r="A769" s="1" t="n">
-        <v>767</v>
-      </c>
-      <c r="B769" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="770">
-      <c r="A770" s="1" t="n">
-        <v>768</v>
-      </c>
-      <c r="B770" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="771">
-      <c r="A771" s="1" t="n">
-        <v>769</v>
-      </c>
-      <c r="B771" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="772">
-      <c r="A772" s="1" t="n">
-        <v>770</v>
-      </c>
-      <c r="B772" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="773">
-      <c r="A773" s="1" t="n">
-        <v>771</v>
-      </c>
-      <c r="B773" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="774">
-      <c r="A774" s="1" t="n">
-        <v>772</v>
-      </c>
-      <c r="B774" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="775">
-      <c r="A775" s="1" t="n">
-        <v>773</v>
-      </c>
-      <c r="B775" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="776">
-      <c r="A776" s="1" t="n">
-        <v>774</v>
-      </c>
-      <c r="B776" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="777">
-      <c r="A777" s="1" t="n">
-        <v>775</v>
-      </c>
-      <c r="B777" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="778">
-      <c r="A778" s="1" t="n">
-        <v>776</v>
-      </c>
-      <c r="B778" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="779">
-      <c r="A779" s="1" t="n">
-        <v>777</v>
-      </c>
-      <c r="B779" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="780">
-      <c r="A780" s="1" t="n">
-        <v>778</v>
-      </c>
-      <c r="B780" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="781">
-      <c r="A781" s="1" t="n">
-        <v>779</v>
-      </c>
-      <c r="B781" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="782">
-      <c r="A782" s="1" t="n">
-        <v>780</v>
-      </c>
-      <c r="B782" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="783">
-      <c r="A783" s="1" t="n">
-        <v>781</v>
-      </c>
-      <c r="B783" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="784">
-      <c r="A784" s="1" t="n">
-        <v>782</v>
-      </c>
-      <c r="B784" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="785">
-      <c r="A785" s="1" t="n">
-        <v>783</v>
-      </c>
-      <c r="B785" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="786">
-      <c r="A786" s="1" t="n">
-        <v>784</v>
-      </c>
-      <c r="B786" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="787">
-      <c r="A787" s="1" t="n">
-        <v>785</v>
-      </c>
-      <c r="B787" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="788">
-      <c r="A788" s="1" t="n">
-        <v>786</v>
-      </c>
-      <c r="B788" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="789">
-      <c r="A789" s="1" t="n">
-        <v>787</v>
-      </c>
-      <c r="B789" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="790">
-      <c r="A790" s="1" t="n">
-        <v>788</v>
-      </c>
-      <c r="B790" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="791">
-      <c r="A791" s="1" t="n">
-        <v>789</v>
-      </c>
-      <c r="B791" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="792">
-      <c r="A792" s="1" t="n">
-        <v>790</v>
-      </c>
-      <c r="B792" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="793">
-      <c r="A793" s="1" t="n">
-        <v>791</v>
-      </c>
-      <c r="B793" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="794">
-      <c r="A794" s="1" t="n">
-        <v>792</v>
-      </c>
-      <c r="B794" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="795">
-      <c r="A795" s="1" t="n">
-        <v>793</v>
-      </c>
-      <c r="B795" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="796">
-      <c r="A796" s="1" t="n">
-        <v>794</v>
-      </c>
-      <c r="B796" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="797">
-      <c r="A797" s="1" t="n">
-        <v>795</v>
-      </c>
-      <c r="B797" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="798">
-      <c r="A798" s="1" t="n">
-        <v>796</v>
-      </c>
-      <c r="B798" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="799">
-      <c r="A799" s="1" t="n">
-        <v>797</v>
-      </c>
-      <c r="B799" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="800">
-      <c r="A800" s="1" t="n">
-        <v>798</v>
-      </c>
-      <c r="B800" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="801">
-      <c r="A801" s="1" t="n">
-        <v>799</v>
-      </c>
-      <c r="B801" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="802">
-      <c r="A802" s="1" t="n">
-        <v>800</v>
-      </c>
-      <c r="B802" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="803">
-      <c r="A803" s="1" t="n">
-        <v>801</v>
-      </c>
-      <c r="B803" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="804">
-      <c r="A804" s="1" t="n">
-        <v>802</v>
-      </c>
-      <c r="B804" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="805">
-      <c r="A805" s="1" t="n">
-        <v>803</v>
-      </c>
-      <c r="B805" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="806">
-      <c r="A806" s="1" t="n">
-        <v>804</v>
-      </c>
-      <c r="B806" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="807">
-      <c r="A807" s="1" t="n">
-        <v>805</v>
-      </c>
-      <c r="B807" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="808">
-      <c r="A808" s="1" t="n">
-        <v>806</v>
-      </c>
-      <c r="B808" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="809">
-      <c r="A809" s="1" t="n">
-        <v>807</v>
-      </c>
-      <c r="B809" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="810">
-      <c r="A810" s="1" t="n">
-        <v>808</v>
-      </c>
-      <c r="B810" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="811">
-      <c r="A811" s="1" t="n">
-        <v>809</v>
-      </c>
-      <c r="B811" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="812">
-      <c r="A812" s="1" t="n">
-        <v>810</v>
-      </c>
-      <c r="B812" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="813">
-      <c r="A813" s="1" t="n">
-        <v>811</v>
-      </c>
-      <c r="B813" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="814">
-      <c r="A814" s="1" t="n">
-        <v>812</v>
-      </c>
-      <c r="B814" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="815">
-      <c r="A815" s="1" t="n">
-        <v>813</v>
-      </c>
-      <c r="B815" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="816">
-      <c r="A816" s="1" t="n">
-        <v>814</v>
-      </c>
-      <c r="B816" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="817">
-      <c r="A817" s="1" t="n">
-        <v>815</v>
-      </c>
-      <c r="B817" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="818">
-      <c r="A818" s="1" t="n">
-        <v>816</v>
-      </c>
-      <c r="B818" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="819">
-      <c r="A819" s="1" t="n">
-        <v>817</v>
-      </c>
-      <c r="B819" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="820">
-      <c r="A820" s="1" t="n">
-        <v>818</v>
-      </c>
-      <c r="B820" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="821">
-      <c r="A821" s="1" t="n">
-        <v>819</v>
-      </c>
-      <c r="B821" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="822">
-      <c r="A822" s="1" t="n">
-        <v>820</v>
-      </c>
-      <c r="B822" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="823">
-      <c r="A823" s="1" t="n">
-        <v>821</v>
-      </c>
-      <c r="B823" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="824">
-      <c r="A824" s="1" t="n">
-        <v>822</v>
-      </c>
-      <c r="B824" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="825">
-      <c r="A825" s="1" t="n">
-        <v>823</v>
-      </c>
-      <c r="B825" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="826">
-      <c r="A826" s="1" t="n">
-        <v>824</v>
-      </c>
-      <c r="B826" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="827">
-      <c r="A827" s="1" t="n">
-        <v>825</v>
-      </c>
-      <c r="B827" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="828">
-      <c r="A828" s="1" t="n">
-        <v>826</v>
-      </c>
-      <c r="B828" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="829">
-      <c r="A829" s="1" t="n">
-        <v>827</v>
-      </c>
-      <c r="B829" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="830">
-      <c r="A830" s="1" t="n">
-        <v>828</v>
-      </c>
-      <c r="B830" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="831">
-      <c r="A831" s="1" t="n">
-        <v>829</v>
-      </c>
-      <c r="B831" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="832">
-      <c r="A832" s="1" t="n">
-        <v>830</v>
-      </c>
-      <c r="B832" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="833">
-      <c r="A833" s="1" t="n">
-        <v>831</v>
-      </c>
-      <c r="B833" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="834">
-      <c r="A834" s="1" t="n">
-        <v>832</v>
-      </c>
-      <c r="B834" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="835">
-      <c r="A835" s="1" t="n">
-        <v>833</v>
-      </c>
-      <c r="B835" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="836">
-      <c r="A836" s="1" t="n">
-        <v>834</v>
-      </c>
-      <c r="B836" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="837">
-      <c r="A837" s="1" t="n">
-        <v>835</v>
-      </c>
-      <c r="B837" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="838">
-      <c r="A838" s="1" t="n">
-        <v>836</v>
-      </c>
-      <c r="B838" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="839">
-      <c r="A839" s="1" t="n">
-        <v>837</v>
-      </c>
-      <c r="B839" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="840">
-      <c r="A840" s="1" t="n">
-        <v>838</v>
-      </c>
-      <c r="B840" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="841">
-      <c r="A841" s="1" t="n">
-        <v>839</v>
-      </c>
-      <c r="B841" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="842">
-      <c r="A842" s="1" t="n">
-        <v>840</v>
-      </c>
-      <c r="B842" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="843">
-      <c r="A843" s="1" t="n">
-        <v>841</v>
-      </c>
-      <c r="B843" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="844">
-      <c r="A844" s="1" t="n">
-        <v>842</v>
-      </c>
-      <c r="B844" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="845">
-      <c r="A845" s="1" t="n">
-        <v>843</v>
-      </c>
-      <c r="B845" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="846">
-      <c r="A846" s="1" t="n">
-        <v>844</v>
-      </c>
-      <c r="B846" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="847">
-      <c r="A847" s="1" t="n">
-        <v>845</v>
-      </c>
-      <c r="B847" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="848">
-      <c r="A848" s="1" t="n">
-        <v>846</v>
-      </c>
-      <c r="B848" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="849">
-      <c r="A849" s="1" t="n">
-        <v>847</v>
-      </c>
-      <c r="B849" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="850">
-      <c r="A850" s="1" t="n">
-        <v>848</v>
-      </c>
-      <c r="B850" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="851">
-      <c r="A851" s="1" t="n">
-        <v>849</v>
-      </c>
-      <c r="B851" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="852">
-      <c r="A852" s="1" t="n">
-        <v>850</v>
-      </c>
-      <c r="B852" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="853">
-      <c r="A853" s="1" t="n">
-        <v>851</v>
-      </c>
-      <c r="B853" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="854">
-      <c r="A854" s="1" t="n">
-        <v>852</v>
-      </c>
-      <c r="B854" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="855">
-      <c r="A855" s="1" t="n">
-        <v>853</v>
-      </c>
-      <c r="B855" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="856">
-      <c r="A856" s="1" t="n">
-        <v>854</v>
-      </c>
-      <c r="B856" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="857">
-      <c r="A857" s="1" t="n">
-        <v>855</v>
-      </c>
-      <c r="B857" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="858">
-      <c r="A858" s="1" t="n">
-        <v>856</v>
-      </c>
-      <c r="B858" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="859">
-      <c r="A859" s="1" t="n">
-        <v>857</v>
-      </c>
-      <c r="B859" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="860">
-      <c r="A860" s="1" t="n">
-        <v>858</v>
-      </c>
-      <c r="B860" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="861">
-      <c r="A861" s="1" t="n">
-        <v>859</v>
-      </c>
-      <c r="B861" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="862">
-      <c r="A862" s="1" t="n">
-        <v>860</v>
-      </c>
-      <c r="B862" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="863">
-      <c r="A863" s="1" t="n">
-        <v>861</v>
-      </c>
-      <c r="B863" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="864">
-      <c r="A864" s="1" t="n">
-        <v>862</v>
-      </c>
-      <c r="B864" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="865">
-      <c r="A865" s="1" t="n">
-        <v>863</v>
-      </c>
-      <c r="B865" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="866">
-      <c r="A866" s="1" t="n">
-        <v>864</v>
-      </c>
-      <c r="B866" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="867">
-      <c r="A867" s="1" t="n">
-        <v>865</v>
-      </c>
-      <c r="B867" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="868">
-      <c r="A868" s="1" t="n">
-        <v>866</v>
-      </c>
-      <c r="B868" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="869">
-      <c r="A869" s="1" t="n">
-        <v>867</v>
-      </c>
-      <c r="B869" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="870">
-      <c r="A870" s="1" t="n">
-        <v>868</v>
-      </c>
-      <c r="B870" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="871">
-      <c r="A871" s="1" t="n">
-        <v>869</v>
-      </c>
-      <c r="B871" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="872">
-      <c r="A872" s="1" t="n">
-        <v>870</v>
-      </c>
-      <c r="B872" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="873">
-      <c r="A873" s="1" t="n">
-        <v>871</v>
-      </c>
-      <c r="B873" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="874">
-      <c r="A874" s="1" t="n">
-        <v>872</v>
-      </c>
-      <c r="B874" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="875">
-      <c r="A875" s="1" t="n">
-        <v>873</v>
-      </c>
-      <c r="B875" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="876">
-      <c r="A876" s="1" t="n">
-        <v>874</v>
-      </c>
-      <c r="B876" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="877">
-      <c r="A877" s="1" t="n">
-        <v>875</v>
-      </c>
-      <c r="B877" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="878">
-      <c r="A878" s="1" t="n">
-        <v>876</v>
-      </c>
-      <c r="B878" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="879">
-      <c r="A879" s="1" t="n">
-        <v>877</v>
-      </c>
-      <c r="B879" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="880">
-      <c r="A880" s="1" t="n">
-        <v>878</v>
-      </c>
-      <c r="B880" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="881">
-      <c r="A881" s="1" t="n">
-        <v>879</v>
-      </c>
-      <c r="B881" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="882">
-      <c r="A882" s="1" t="n">
-        <v>880</v>
-      </c>
-      <c r="B882" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="883">
-      <c r="A883" s="1" t="n">
-        <v>881</v>
-      </c>
-      <c r="B883" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="884">
-      <c r="A884" s="1" t="n">
-        <v>882</v>
-      </c>
-      <c r="B884" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="885">
-      <c r="A885" s="1" t="n">
-        <v>883</v>
-      </c>
-      <c r="B885" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="886">
-      <c r="A886" s="1" t="n">
-        <v>884</v>
-      </c>
-      <c r="B886" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="887">
-      <c r="A887" s="1" t="n">
-        <v>885</v>
-      </c>
-      <c r="B887" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="888">
-      <c r="A888" s="1" t="n">
-        <v>886</v>
-      </c>
-      <c r="B888" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="889">
-      <c r="A889" s="1" t="n">
-        <v>887</v>
-      </c>
-      <c r="B889" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="890">
-      <c r="A890" s="1" t="n">
-        <v>888</v>
-      </c>
-      <c r="B890" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="891">
-      <c r="A891" s="1" t="n">
-        <v>889</v>
-      </c>
-      <c r="B891" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="892">
-      <c r="A892" s="1" t="n">
-        <v>890</v>
-      </c>
-      <c r="B892" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="893">
-      <c r="A893" s="1" t="n">
-        <v>891</v>
-      </c>
-      <c r="B893" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="894">
-      <c r="A894" s="1" t="n">
-        <v>892</v>
-      </c>
-      <c r="B894" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="895">
-      <c r="A895" s="1" t="n">
-        <v>893</v>
-      </c>
-      <c r="B895" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>